<commit_message>
Added codes for heston callibration
</commit_message>
<xml_diff>
--- a/BABA 3M Equity.xlsx
+++ b/BABA 3M Equity.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19330"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Novdano\Desktop\SURF\Option-Pricing\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A58193E6-1F5E-4072-9B15-0D10028BE10F}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -498,7 +504,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -541,6 +547,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -589,7 +598,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -622,9 +631,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -657,6 +683,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -832,20 +875,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E95"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="2" width="14.28515625" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="14.26171875" customWidth="1"/>
+    <col min="3" max="3" width="18.68359375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -859,7 +902,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -876,7 +919,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -893,7 +936,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -910,7 +953,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -927,7 +970,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -944,7 +987,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -961,7 +1004,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -978,10 +1021,10 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" s="1"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -998,7 +1041,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1015,7 +1058,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -1032,7 +1075,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -1049,7 +1092,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -1066,10 +1109,10 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B16" s="1"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -1086,7 +1129,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>11</v>
       </c>
@@ -1103,7 +1146,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -1120,7 +1163,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>2</v>
       </c>
@@ -1137,7 +1180,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>5</v>
       </c>
@@ -1154,10 +1197,10 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B22" s="1"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>8</v>
       </c>
@@ -1174,7 +1217,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>11</v>
       </c>
@@ -1191,7 +1234,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
         <v>14</v>
       </c>
@@ -1208,7 +1251,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
         <v>2</v>
       </c>
@@ -1225,10 +1268,10 @@
         <v>48</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B27" s="1"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
         <v>8</v>
       </c>
@@ -1245,7 +1288,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
         <v>11</v>
       </c>
@@ -1262,7 +1305,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
         <v>14</v>
       </c>
@@ -1279,7 +1322,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
         <v>2</v>
       </c>
@@ -1296,7 +1339,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
         <v>5</v>
       </c>
@@ -1313,7 +1356,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
         <v>8</v>
       </c>
@@ -1330,7 +1373,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
         <v>11</v>
       </c>
@@ -1347,7 +1390,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
         <v>14</v>
       </c>
@@ -1364,7 +1407,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
         <v>2</v>
       </c>
@@ -1381,7 +1424,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
         <v>5</v>
       </c>
@@ -1398,7 +1441,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
         <v>8</v>
       </c>
@@ -1415,7 +1458,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
         <v>11</v>
       </c>
@@ -1432,7 +1475,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
         <v>14</v>
       </c>
@@ -1449,7 +1492,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
         <v>2</v>
       </c>
@@ -1466,7 +1509,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
         <v>5</v>
       </c>
@@ -1483,7 +1526,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
         <v>8</v>
       </c>
@@ -1500,7 +1543,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
         <v>11</v>
       </c>
@@ -1517,7 +1560,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" t="s">
         <v>14</v>
       </c>
@@ -1534,7 +1577,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" t="s">
         <v>2</v>
       </c>
@@ -1551,7 +1594,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" t="s">
         <v>5</v>
       </c>
@@ -1568,7 +1611,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" t="s">
         <v>8</v>
       </c>
@@ -1585,7 +1628,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" t="s">
         <v>11</v>
       </c>
@@ -1602,7 +1645,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" t="s">
         <v>14</v>
       </c>
@@ -1619,7 +1662,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" t="s">
         <v>2</v>
       </c>
@@ -1636,7 +1679,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" t="s">
         <v>5</v>
       </c>
@@ -1653,7 +1696,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" t="s">
         <v>8</v>
       </c>
@@ -1670,7 +1713,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" t="s">
         <v>11</v>
       </c>
@@ -1687,7 +1730,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" t="s">
         <v>14</v>
       </c>
@@ -1704,7 +1747,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" t="s">
         <v>2</v>
       </c>
@@ -1721,7 +1764,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" t="s">
         <v>5</v>
       </c>
@@ -1738,7 +1781,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" t="s">
         <v>8</v>
       </c>
@@ -1755,7 +1798,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" t="s">
         <v>11</v>
       </c>
@@ -1772,7 +1815,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" t="s">
         <v>14</v>
       </c>
@@ -1789,7 +1832,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" t="s">
         <v>2</v>
       </c>
@@ -1806,7 +1849,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" t="s">
         <v>5</v>
       </c>
@@ -1823,7 +1866,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" t="s">
         <v>8</v>
       </c>
@@ -1840,7 +1883,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" t="s">
         <v>11</v>
       </c>
@@ -1857,7 +1900,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" t="s">
         <v>14</v>
       </c>
@@ -1874,7 +1917,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" t="s">
         <v>2</v>
       </c>
@@ -1891,7 +1934,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" t="s">
         <v>5</v>
       </c>
@@ -1908,7 +1951,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" t="s">
         <v>11</v>
       </c>
@@ -1925,7 +1968,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" t="s">
         <v>14</v>
       </c>
@@ -1942,7 +1985,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" t="s">
         <v>2</v>
       </c>
@@ -1959,7 +2002,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" t="s">
         <v>5</v>
       </c>
@@ -1973,7 +2016,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" t="s">
         <v>8</v>
       </c>
@@ -1987,7 +2030,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" t="s">
         <v>11</v>
       </c>
@@ -2001,7 +2044,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" t="s">
         <v>14</v>
       </c>
@@ -2015,7 +2058,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" t="s">
         <v>2</v>
       </c>
@@ -2029,7 +2072,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" t="s">
         <v>5</v>
       </c>
@@ -2043,7 +2086,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" t="s">
         <v>8</v>
       </c>
@@ -2057,7 +2100,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" t="s">
         <v>11</v>
       </c>
@@ -2071,7 +2114,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" t="s">
         <v>14</v>
       </c>
@@ -2085,7 +2128,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" t="s">
         <v>2</v>
       </c>
@@ -2099,7 +2142,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" t="s">
         <v>5</v>
       </c>
@@ -2113,7 +2156,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" t="s">
         <v>8</v>
       </c>
@@ -2127,7 +2170,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" t="s">
         <v>11</v>
       </c>
@@ -2141,7 +2184,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" t="s">
         <v>14</v>
       </c>
@@ -2162,20 +2205,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:R182"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="2" width="17.140625" customWidth="1"/>
-    <col min="18" max="18" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.15625" customWidth="1"/>
+    <col min="18" max="18" width="9.68359375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -2210,7 +2253,7 @@
         <v>43301</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -2242,7 +2285,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -2274,7 +2317,7 @@
         <v>28500</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -2306,7 +2349,7 @@
         <v>27522</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -2338,7 +2381,7 @@
         <v>26755</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -2370,7 +2413,7 @@
         <v>25985</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -2402,7 +2445,7 @@
         <v>25137</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -2434,7 +2477,7 @@
         <v>24213</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -2466,7 +2509,7 @@
         <v>23201</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -2498,7 +2541,7 @@
         <v>22067</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -2530,7 +2573,7 @@
         <v>21002</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -2562,7 +2605,7 @@
         <v>20241</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -2594,7 +2637,7 @@
         <v>19478</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -2626,7 +2669,7 @@
         <v>18713</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>11</v>
       </c>
@@ -2658,7 +2701,7 @@
         <v>17913</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -2690,7 +2733,7 @@
         <v>17116</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>2</v>
       </c>
@@ -2722,7 +2765,7 @@
         <v>16391</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>5</v>
       </c>
@@ -2754,7 +2797,7 @@
         <v>15819</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>8</v>
       </c>
@@ -2786,7 +2829,7 @@
         <v>15187</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>11</v>
       </c>
@@ -2818,7 +2861,7 @@
         <v>14541</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
         <v>14</v>
       </c>
@@ -2850,7 +2893,7 @@
         <v>13913</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
         <v>2</v>
       </c>
@@ -2882,7 +2925,7 @@
         <v>13391</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
         <v>8</v>
       </c>
@@ -2914,7 +2957,7 @@
         <v>12917</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
         <v>11</v>
       </c>
@@ -2946,7 +2989,7 @@
         <v>12625</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
         <v>14</v>
       </c>
@@ -2978,7 +3021,7 @@
         <v>12501</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
         <v>2</v>
       </c>
@@ -3010,7 +3053,7 @@
         <v>12488</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
         <v>5</v>
       </c>
@@ -3042,7 +3085,7 @@
         <v>12329</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
         <v>8</v>
       </c>
@@ -3074,7 +3117,7 @@
         <v>12152</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
         <v>11</v>
       </c>
@@ -3106,7 +3149,7 @@
         <v>11968</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
         <v>14</v>
       </c>
@@ -3138,7 +3181,7 @@
         <v>11808</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
         <v>2</v>
       </c>
@@ -3170,7 +3213,7 @@
         <v>11628</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
         <v>5</v>
       </c>
@@ -3202,7 +3245,7 @@
         <v>11450</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
         <v>8</v>
       </c>
@@ -3234,7 +3277,7 @@
         <v>11298</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
         <v>11</v>
       </c>
@@ -3266,7 +3309,7 @@
         <v>11148</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
         <v>14</v>
       </c>
@@ -3298,7 +3341,7 @@
         <v>10988</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
         <v>2</v>
       </c>
@@ -3330,7 +3373,7 @@
         <v>10686</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
         <v>5</v>
       </c>
@@ -3362,7 +3405,7 @@
         <v>10371</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
         <v>8</v>
       </c>
@@ -3394,7 +3437,7 @@
         <v>10058</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
         <v>11</v>
       </c>
@@ -3426,7 +3469,7 @@
         <v>9658</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" t="s">
         <v>14</v>
       </c>
@@ -3458,7 +3501,7 @@
         <v>9281</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" t="s">
         <v>2</v>
       </c>
@@ -3490,7 +3533,7 @@
         <v>8955</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" t="s">
         <v>5</v>
       </c>
@@ -3522,7 +3565,7 @@
         <v>8765</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" t="s">
         <v>8</v>
       </c>
@@ -3554,7 +3597,7 @@
         <v>8582</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" t="s">
         <v>11</v>
       </c>
@@ -3586,7 +3629,7 @@
         <v>8405</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" t="s">
         <v>14</v>
       </c>
@@ -3618,7 +3661,7 @@
         <v>8236</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" t="s">
         <v>2</v>
       </c>
@@ -3650,7 +3693,7 @@
         <v>8081</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" t="s">
         <v>5</v>
       </c>
@@ -3682,7 +3725,7 @@
         <v>7894</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" t="s">
         <v>8</v>
       </c>
@@ -3714,7 +3757,7 @@
         <v>7710</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" t="s">
         <v>11</v>
       </c>
@@ -3746,7 +3789,7 @@
         <v>7530</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" t="s">
         <v>14</v>
       </c>
@@ -3778,7 +3821,7 @@
         <v>7352</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" t="s">
         <v>2</v>
       </c>
@@ -3810,7 +3853,7 @@
         <v>7301</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" t="s">
         <v>5</v>
       </c>
@@ -3839,7 +3882,7 @@
         <v>7256</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" t="s">
         <v>8</v>
       </c>
@@ -3868,7 +3911,7 @@
         <v>7208</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" t="s">
         <v>11</v>
       </c>
@@ -3897,7 +3940,7 @@
         <v>7082</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" t="s">
         <v>14</v>
       </c>
@@ -3926,7 +3969,7 @@
         <v>6948</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" t="s">
         <v>2</v>
       </c>
@@ -3955,7 +3998,7 @@
         <v>6829</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" t="s">
         <v>5</v>
       </c>
@@ -3984,7 +4027,7 @@
         <v>6709</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" t="s">
         <v>8</v>
       </c>
@@ -4013,7 +4056,7 @@
         <v>6590</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" t="s">
         <v>11</v>
       </c>
@@ -4042,7 +4085,7 @@
         <v>6471</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" t="s">
         <v>14</v>
       </c>
@@ -4071,7 +4114,7 @@
         <v>6357</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" t="s">
         <v>2</v>
       </c>
@@ -4100,7 +4143,7 @@
         <v>6253</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" t="s">
         <v>5</v>
       </c>
@@ -4129,7 +4172,7 @@
         <v>6136</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" t="s">
         <v>11</v>
       </c>
@@ -4158,7 +4201,7 @@
         <v>6047</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" t="s">
         <v>14</v>
       </c>
@@ -4187,7 +4230,7 @@
         <v>5962</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" t="s">
         <v>2</v>
       </c>
@@ -4216,7 +4259,7 @@
         <v>5890</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" t="s">
         <v>5</v>
       </c>
@@ -4245,7 +4288,7 @@
         <v>5823</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" t="s">
         <v>8</v>
       </c>
@@ -4274,7 +4317,7 @@
         <v>5755</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" t="s">
         <v>11</v>
       </c>
@@ -4303,7 +4346,7 @@
         <v>5685</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" t="s">
         <v>14</v>
       </c>
@@ -4332,7 +4375,7 @@
         <v>5693</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" t="s">
         <v>2</v>
       </c>
@@ -4361,7 +4404,7 @@
         <v>5717</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" t="s">
         <v>5</v>
       </c>
@@ -4390,7 +4433,7 @@
         <v>5707</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" t="s">
         <v>8</v>
       </c>
@@ -4419,7 +4462,7 @@
         <v>5670</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" t="s">
         <v>11</v>
       </c>
@@ -4448,7 +4491,7 @@
         <v>5635</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" t="s">
         <v>14</v>
       </c>
@@ -4477,7 +4520,7 @@
         <v>5601</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" t="s">
         <v>2</v>
       </c>
@@ -4506,7 +4549,7 @@
         <v>5562</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" t="s">
         <v>5</v>
       </c>
@@ -4535,7 +4578,7 @@
         <v>5519</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" t="s">
         <v>8</v>
       </c>
@@ -4564,7 +4607,7 @@
         <v>5495</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" t="s">
         <v>11</v>
       </c>
@@ -4593,7 +4636,7 @@
         <v>5448</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" t="s">
         <v>14</v>
       </c>
@@ -4622,7 +4665,7 @@
         <v>5395</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" t="s">
         <v>2</v>
       </c>
@@ -4651,7 +4694,7 @@
         <v>5332</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" t="s">
         <v>5</v>
       </c>
@@ -4680,7 +4723,7 @@
         <v>5259</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" t="s">
         <v>8</v>
       </c>
@@ -4709,7 +4752,7 @@
         <v>5185</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" t="s">
         <v>11</v>
       </c>
@@ -4738,7 +4781,7 @@
         <v>5123</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" t="s">
         <v>14</v>
       </c>
@@ -4767,7 +4810,7 @@
         <v>5070</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A102" t="s">
         <v>2</v>
       </c>
@@ -4796,7 +4839,7 @@
         <v>5013</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A103" t="s">
         <v>5</v>
       </c>
@@ -4825,7 +4868,7 @@
         <v>4979</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" t="s">
         <v>8</v>
       </c>
@@ -4854,7 +4897,7 @@
         <v>4965</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" t="s">
         <v>11</v>
       </c>
@@ -4883,7 +4926,7 @@
         <v>4937</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A107" t="s">
         <v>14</v>
       </c>
@@ -4912,7 +4955,7 @@
         <v>4889</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A108" t="s">
         <v>2</v>
       </c>
@@ -4941,7 +4984,7 @@
         <v>4839</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A110" t="s">
         <v>8</v>
       </c>
@@ -4970,7 +5013,7 @@
         <v>4785</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A111" t="s">
         <v>11</v>
       </c>
@@ -4999,7 +5042,7 @@
         <v>4735</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A112" t="s">
         <v>14</v>
       </c>
@@ -5028,7 +5071,7 @@
         <v>4668</v>
       </c>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A113" t="s">
         <v>2</v>
       </c>
@@ -5057,7 +5100,7 @@
         <v>4591</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A114" t="s">
         <v>5</v>
       </c>
@@ -5086,7 +5129,7 @@
         <v>4512</v>
       </c>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A116" t="s">
         <v>8</v>
       </c>
@@ -5115,7 +5158,7 @@
         <v>4445</v>
       </c>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A117" t="s">
         <v>11</v>
       </c>
@@ -5144,7 +5187,7 @@
         <v>4376</v>
       </c>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A118" t="s">
         <v>14</v>
       </c>
@@ -5173,7 +5216,7 @@
         <v>4300</v>
       </c>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A119" t="s">
         <v>2</v>
       </c>
@@ -5202,7 +5245,7 @@
         <v>4212</v>
       </c>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A120" t="s">
         <v>5</v>
       </c>
@@ -5231,7 +5274,7 @@
         <v>4121</v>
       </c>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A122" t="s">
         <v>8</v>
       </c>
@@ -5260,7 +5303,7 @@
         <v>4004</v>
       </c>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A123" t="s">
         <v>11</v>
       </c>
@@ -5286,7 +5329,7 @@
         <v>3886</v>
       </c>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A124" t="s">
         <v>14</v>
       </c>
@@ -5312,7 +5355,7 @@
         <v>3776</v>
       </c>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A125" t="s">
         <v>2</v>
       </c>
@@ -5338,7 +5381,7 @@
         <v>3680</v>
       </c>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A126" t="s">
         <v>5</v>
       </c>
@@ -5364,7 +5407,7 @@
         <v>3559</v>
       </c>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A128" t="s">
         <v>8</v>
       </c>
@@ -5390,7 +5433,7 @@
         <v>3432</v>
       </c>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A129" t="s">
         <v>11</v>
       </c>
@@ -5416,7 +5459,7 @@
         <v>3267</v>
       </c>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A130" t="s">
         <v>14</v>
       </c>
@@ -5442,7 +5485,7 @@
         <v>3120</v>
       </c>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A131" t="s">
         <v>2</v>
       </c>
@@ -5468,7 +5511,7 @@
         <v>2964</v>
       </c>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A132" t="s">
         <v>5</v>
       </c>
@@ -5494,7 +5537,7 @@
         <v>2810</v>
       </c>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A134" t="s">
         <v>8</v>
       </c>
@@ -5520,7 +5563,7 @@
         <v>2648</v>
       </c>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A135" t="s">
         <v>11</v>
       </c>
@@ -5546,7 +5589,7 @@
         <v>2491</v>
       </c>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A136" t="s">
         <v>14</v>
       </c>
@@ -5572,7 +5615,7 @@
         <v>2338</v>
       </c>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A137" t="s">
         <v>2</v>
       </c>
@@ -5598,7 +5641,7 @@
         <v>2187</v>
       </c>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A139" t="s">
         <v>8</v>
       </c>
@@ -5624,7 +5667,7 @@
         <v>2038</v>
       </c>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A140" t="s">
         <v>11</v>
       </c>
@@ -5650,7 +5693,7 @@
         <v>1927</v>
       </c>
     </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A141" t="s">
         <v>14</v>
       </c>
@@ -5676,7 +5719,7 @@
         <v>1751</v>
       </c>
     </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A142" t="s">
         <v>2</v>
       </c>
@@ -5702,7 +5745,7 @@
         <v>1579</v>
       </c>
     </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A143" t="s">
         <v>5</v>
       </c>
@@ -5728,7 +5771,7 @@
         <v>1414</v>
       </c>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A145" t="s">
         <v>8</v>
       </c>
@@ -5754,7 +5797,7 @@
         <v>1275</v>
       </c>
     </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A146" t="s">
         <v>11</v>
       </c>
@@ -5780,7 +5823,7 @@
         <v>1144</v>
       </c>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A147" t="s">
         <v>14</v>
       </c>
@@ -5806,7 +5849,7 @@
         <v>1049</v>
       </c>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A148" t="s">
         <v>2</v>
       </c>
@@ -5832,7 +5875,7 @@
         <v>953</v>
       </c>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A150" t="s">
         <v>8</v>
       </c>
@@ -5858,7 +5901,7 @@
         <v>868</v>
       </c>
     </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A151" t="s">
         <v>11</v>
       </c>
@@ -5884,7 +5927,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A152" t="s">
         <v>14</v>
       </c>
@@ -5910,7 +5953,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A153" t="s">
         <v>2</v>
       </c>
@@ -5936,7 +5979,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A155" t="s">
         <v>8</v>
       </c>
@@ -5962,7 +6005,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A156" t="s">
         <v>11</v>
       </c>
@@ -5988,7 +6031,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A157" t="s">
         <v>14</v>
       </c>
@@ -6014,7 +6057,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A158" t="s">
         <v>2</v>
       </c>
@@ -6040,7 +6083,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A159" t="s">
         <v>5</v>
       </c>
@@ -6066,7 +6109,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A161" t="s">
         <v>8</v>
       </c>
@@ -6092,7 +6135,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A162" t="s">
         <v>11</v>
       </c>
@@ -6106,7 +6149,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A163" t="s">
         <v>14</v>
       </c>
@@ -6132,7 +6175,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A164" t="s">
         <v>2</v>
       </c>
@@ -6158,7 +6201,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A165" t="s">
         <v>5</v>
       </c>
@@ -6184,7 +6227,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A167" t="s">
         <v>8</v>
       </c>
@@ -6207,7 +6250,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A168" t="s">
         <v>11</v>
       </c>
@@ -6230,7 +6273,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A169" t="s">
         <v>14</v>
       </c>
@@ -6253,7 +6296,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A170" t="s">
         <v>2</v>
       </c>
@@ -6276,7 +6319,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A171" t="s">
         <v>5</v>
       </c>
@@ -6299,7 +6342,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A173" t="s">
         <v>8</v>
       </c>
@@ -6322,7 +6365,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="174" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A174" t="s">
         <v>11</v>
       </c>
@@ -6345,7 +6388,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="175" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A175" t="s">
         <v>14</v>
       </c>
@@ -6368,7 +6411,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="176" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A176" t="s">
         <v>2</v>
       </c>
@@ -6391,7 +6434,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A177" t="s">
         <v>5</v>
       </c>
@@ -6414,7 +6457,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A179" t="s">
         <v>8</v>
       </c>
@@ -6437,7 +6480,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A180" t="s">
         <v>14</v>
       </c>
@@ -6460,7 +6503,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A181" t="s">
         <v>2</v>
       </c>
@@ -6483,7 +6526,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A182" t="s">
         <v>5</v>
       </c>
@@ -6512,20 +6555,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:O34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="3" width="11.42578125" customWidth="1"/>
-    <col min="15" max="15" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="11.41796875" customWidth="1"/>
+    <col min="15" max="15" width="9.68359375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -6560,7 +6603,7 @@
         <v>43364</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -6586,7 +6629,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -6612,7 +6655,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -6638,7 +6681,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -6664,7 +6707,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -6690,7 +6733,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -6716,7 +6759,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -6742,7 +6785,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -6768,7 +6811,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -6794,7 +6837,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -6820,7 +6863,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -6846,7 +6889,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -6872,7 +6915,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -6898,7 +6941,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>11</v>
       </c>
@@ -6921,7 +6964,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -6944,7 +6987,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>2</v>
       </c>
@@ -6967,7 +7010,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>5</v>
       </c>
@@ -6990,7 +7033,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>8</v>
       </c>
@@ -7013,7 +7056,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>11</v>
       </c>
@@ -7036,7 +7079,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
         <v>14</v>
       </c>
@@ -7059,7 +7102,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
         <v>2</v>
       </c>
@@ -7082,7 +7125,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
         <v>8</v>
       </c>
@@ -7105,7 +7148,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
         <v>11</v>
       </c>
@@ -7128,7 +7171,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
         <v>14</v>
       </c>
@@ -7151,7 +7194,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
         <v>2</v>
       </c>
@@ -7174,7 +7217,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
         <v>5</v>
       </c>
@@ -7197,7 +7240,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
         <v>8</v>
       </c>

</xml_diff>